<commit_message>
Another day of data scraped. Geodata not updated yet for prior week.
</commit_message>
<xml_diff>
--- a/ilimapper.xlsx
+++ b/ilimapper.xlsx
@@ -27,7 +27,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="pctresp.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:david:Desktop:ilimapper:output:phu_pctresp.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:david:Documents:projects:ilimapper:output:phu_pctresp.csv" tab="0" comma="1">
       <textFields count="34">
         <textField/>
         <textField/>
@@ -109,7 +109,7 @@
     </textPr>
   </connection>
   <connection id="3" name="respvisits.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="Macintosh HD:Users:david:Desktop:ilimapper:output:phu_respvisits.csv" comma="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:david:Documents:projects:ilimapper:output:phu_respvisits.csv" comma="1">
       <textFields count="34">
         <textField/>
         <textField/>
@@ -3171,11 +3171,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2067326360"/>
-        <c:axId val="2067320488"/>
+        <c:axId val="2069309624"/>
+        <c:axId val="2069312712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2067326360"/>
+        <c:axId val="2069309624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3195,7 +3195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2067320488"/>
+        <c:crossAx val="2069312712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -3204,7 +3204,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2067320488"/>
+        <c:axId val="2069312712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3242,7 +3242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067326360"/>
+        <c:crossAx val="2069309624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3635,38 +3635,29 @@
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF2" sqref="AF2"/>
+      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="9" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22511,38 +22502,29 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AA2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH3" sqref="AH3"/>
+      <selection pane="bottomRight" activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="9" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41384,7 +41366,7 @@
   <dimension ref="A1:V182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="133" topLeftCell="B177" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="133" topLeftCell="B173" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="A133" sqref="A3:XFD133"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>

</xml_diff>